<commit_message>
Changes in the xls
</commit_message>
<xml_diff>
--- a/xlsx/Population/KP_WSF_adm3_Pop.xlsx
+++ b/xlsx/Population/KP_WSF_adm3_Pop.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/shaider7_worldbank_org/Documents/Documents/WB_FY2023/KPK Population Growth Analysis/KP_Pop_ServiceAccessibility_Project/xlsx/Population/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb578340\OneDrive - WBG\Documents\WB_FY2023\KPK Population Growth Analysis\KP_Pop_ServiceAccessibility_Project\xlsx\Population\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8070C8B1-0021-401D-B2A5-E4C411D53DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EDE811F-8550-4D19-BEE2-B699036A2286}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F69BF60-8BE5-4BDD-8523-93D7E7810077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="413">
   <si>
     <t>ADM3_NAME</t>
   </si>
@@ -1294,18 +1294,6 @@
   </si>
   <si>
     <t>WPOP20_Pop_density/sqkm_2030</t>
-  </si>
-  <si>
-    <t>Primary schools per capita</t>
-  </si>
-  <si>
-    <t>Hospitals per capita</t>
-  </si>
-  <si>
-    <t>Police Stations Per capita</t>
-  </si>
-  <si>
-    <t>1% increase in KP</t>
   </si>
 </sst>
 </file>
@@ -2234,8 +2222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156:XFD165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15281,46 +15269,19 @@
       <c r="X155" s="19"/>
     </row>
     <row r="158" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="J158" t="s">
-        <v>416</v>
-      </c>
-      <c r="K158" s="22">
-        <f>K155*1.01</f>
-        <v>34133625.689999998</v>
-      </c>
+      <c r="K158" s="22"/>
     </row>
     <row r="159" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="K159" s="1">
-        <f>K158-K155</f>
-        <v>337956.68999999762</v>
-      </c>
+      <c r="K159" s="1"/>
     </row>
     <row r="160" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="J160" t="s">
-        <v>413</v>
-      </c>
-      <c r="K160" s="22">
-        <f>K159/21</f>
-        <v>16093.1757142856</v>
-      </c>
-    </row>
-    <row r="161" spans="10:11" x14ac:dyDescent="0.35">
-      <c r="J161" t="s">
-        <v>414</v>
-      </c>
-      <c r="K161" s="22">
-        <f>K159/3</f>
-        <v>112652.22999999921</v>
-      </c>
-    </row>
-    <row r="162" spans="10:11" x14ac:dyDescent="0.35">
-      <c r="J162" t="s">
-        <v>415</v>
-      </c>
-      <c r="K162" s="22">
-        <f>K159/2</f>
-        <v>168978.34499999881</v>
-      </c>
+      <c r="K160" s="22"/>
+    </row>
+    <row r="161" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K161" s="22"/>
+    </row>
+    <row r="162" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K162" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final changes for version 5
</commit_message>
<xml_diff>
--- a/xlsx/Population/KP_WSF_adm3_Pop.xlsx
+++ b/xlsx/Population/KP_WSF_adm3_Pop.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb578340\OneDrive - WBG\Documents\WB_FY2023\KPK Population Growth Analysis\KP_Pop_ServiceAccessibility_Project\xlsx\Population\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/shaider7_worldbank_org/Documents/Documents/WB_FY2023/KPK Population Growth Analysis/KP_Pop_ServiceAccessibility_Project/xlsx/Population/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F69BF60-8BE5-4BDD-8523-93D7E7810077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -2222,8 +2222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156:XFD165"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>